<commit_message>
adjusted excel file handling
</commit_message>
<xml_diff>
--- a/demo/extended_inventory_demo.xlsx
+++ b/demo/extended_inventory_demo.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arpit\Desktop\Sociothon24_AI-FoodWasteReduction\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F6FF2-614D-48DA-B499-5AB478CF4AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -118,11 +124,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,13 +192,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +244,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -264,6 +278,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -298,9 +313,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,14 +489,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="I138" sqref="I138"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -499,10 +520,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>45570.48804522204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>45570.488045222039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -510,10 +531,10 @@
         <v>20</v>
       </c>
       <c r="C3" s="2">
-        <v>45582.4880452222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>45582.488045222199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -521,10 +542,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="2">
-        <v>45579.48804522224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>45579.488045222242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -532,10 +553,10 @@
         <v>46</v>
       </c>
       <c r="C5" s="2">
-        <v>45571.48804522229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>45571.488045222293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -543,10 +564,10 @@
         <v>48</v>
       </c>
       <c r="C6" s="2">
-        <v>45590.48804522234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>45590.488045222337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -554,10 +575,10 @@
         <v>37</v>
       </c>
       <c r="C7" s="2">
-        <v>45578.48804522239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>45578.488045222388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -565,10 +586,10 @@
         <v>48</v>
       </c>
       <c r="C8" s="2">
-        <v>45583.48804522243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>45583.488045222432</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -579,7 +600,7 @@
         <v>45574.48804522249</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -587,10 +608,10 @@
         <v>29</v>
       </c>
       <c r="C10" s="2">
-        <v>45585.48804522255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>45585.488045222548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -598,10 +619,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>45586.48804522259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>45586.488045222592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -609,10 +630,10 @@
         <v>42</v>
       </c>
       <c r="C12" s="2">
-        <v>45570.48804522264</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>45570.488045222643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -620,10 +641,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="2">
-        <v>45576.48804522269</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>45576.488045222693</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -631,10 +652,10 @@
         <v>50</v>
       </c>
       <c r="C14" s="2">
-        <v>45562.48804522272</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>45562.488045222723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -642,10 +663,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="2">
-        <v>45573.48804522277</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>45573.488045222774</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -653,10 +674,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="2">
-        <v>45573.4880452228</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>45573.488045222803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -664,10 +685,10 @@
         <v>24</v>
       </c>
       <c r="C17" s="2">
-        <v>45569.48804522285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>45569.488045222854</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -675,10 +696,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>45586.48804522288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>45586.488045222883</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -686,10 +707,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="2">
-        <v>45564.48804522293</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>45564.488045222934</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -697,10 +718,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="2">
-        <v>45589.48804522296</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>45589.488045222963</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -708,10 +729,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="2">
-        <v>45580.48804522301</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>45580.488045223014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -719,10 +740,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="2">
-        <v>45577.48804522306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>45577.488045223057</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -730,10 +751,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>45568.48804522309</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>45568.488045223086</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -741,10 +762,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="2">
-        <v>45561.48804522314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>45561.488045223137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -752,10 +773,10 @@
         <v>16</v>
       </c>
       <c r="C25" s="2">
-        <v>45582.48804522317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>45582.488045223166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -763,10 +784,10 @@
         <v>13</v>
       </c>
       <c r="C26" s="2">
-        <v>45567.48804522322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>45567.488045223217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -774,10 +795,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="2">
-        <v>45568.48804522326</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>45568.488045223261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -785,10 +806,10 @@
         <v>31</v>
       </c>
       <c r="C28" s="2">
-        <v>45582.48804522331</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>45582.488045223312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -796,10 +817,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="2">
-        <v>45580.48804522335</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>45580.488045223348</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -807,10 +828,10 @@
         <v>19</v>
       </c>
       <c r="C30" s="2">
-        <v>45571.48804522338</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>45571.488045223377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -818,10 +839,10 @@
         <v>40</v>
       </c>
       <c r="C31" s="2">
-        <v>45567.48804522341</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>45567.488045223407</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -829,10 +850,10 @@
         <v>47</v>
       </c>
       <c r="C32" s="2">
-        <v>45570.48804522346</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>45570.488045223457</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -840,10 +861,10 @@
         <v>40</v>
       </c>
       <c r="C33" s="2">
-        <v>45575.48804522349</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>45575.488045223487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -851,10 +872,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="2">
-        <v>45564.48804522354</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>45564.488045223537</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -862,10 +883,10 @@
         <v>22</v>
       </c>
       <c r="C35" s="2">
-        <v>45582.48804522359</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>45582.488045223588</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -873,10 +894,10 @@
         <v>6</v>
       </c>
       <c r="C36" s="2">
-        <v>45563.48804522362</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>45563.488045223618</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -884,10 +905,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="2">
-        <v>45566.48804522367</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>45566.488045223668</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -895,10 +916,10 @@
         <v>35</v>
       </c>
       <c r="C38" s="2">
-        <v>45583.48804522371</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>45583.488045223712</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -906,10 +927,10 @@
         <v>47</v>
       </c>
       <c r="C39" s="2">
-        <v>45578.48804522375</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>45578.488045223748</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -917,10 +938,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="2">
-        <v>45580.48804522378</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>45580.488045223778</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -928,10 +949,10 @@
         <v>22</v>
       </c>
       <c r="C41" s="2">
-        <v>45562.48804522383</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>45562.488045223829</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -939,10 +960,10 @@
         <v>2</v>
       </c>
       <c r="C42" s="2">
-        <v>45587.48804522386</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>45587.488045223858</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -950,10 +971,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="2">
-        <v>45573.48804522391</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>45573.488045223909</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -961,10 +982,10 @@
         <v>48</v>
       </c>
       <c r="C44" s="2">
-        <v>45587.48804522394</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>45587.488045223938</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -972,10 +993,10 @@
         <v>45</v>
       </c>
       <c r="C45" s="2">
-        <v>45575.488045224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>45575.488045224003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -983,10 +1004,10 @@
         <v>28</v>
       </c>
       <c r="C46" s="2">
-        <v>45569.48804522402</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>45569.488045224018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -994,10 +1015,10 @@
         <v>42</v>
       </c>
       <c r="C47" s="2">
-        <v>45571.48804522408</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>45571.488045224083</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1005,10 +1026,10 @@
         <v>44</v>
       </c>
       <c r="C48" s="2">
-        <v>45561.48804522411</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>45561.488045224112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1016,10 +1037,10 @@
         <v>41</v>
       </c>
       <c r="C49" s="2">
-        <v>45573.48804522427</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>45573.488045224272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1027,10 +1048,10 @@
         <v>20</v>
       </c>
       <c r="C50" s="2">
-        <v>45566.48804522432</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>45566.488045224323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1038,10 +1059,10 @@
         <v>29</v>
       </c>
       <c r="C51" s="2">
-        <v>45578.48804522435</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>45578.488045224352</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -1049,10 +1070,10 @@
         <v>42</v>
       </c>
       <c r="C52" s="2">
-        <v>45566.4880452244</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>45566.488045224403</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -1060,10 +1081,10 @@
         <v>12</v>
       </c>
       <c r="C53" s="2">
-        <v>45568.48804522443</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>45568.488045224432</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -1071,10 +1092,10 @@
         <v>44</v>
       </c>
       <c r="C54" s="2">
-        <v>45580.48804522448</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>45580.488045224483</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -1082,10 +1103,10 @@
         <v>4</v>
       </c>
       <c r="C55" s="2">
-        <v>45590.48804522453</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>45590.488045224527</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1093,10 +1114,10 @@
         <v>42</v>
       </c>
       <c r="C56" s="2">
-        <v>45571.48804522456</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>45571.488045224563</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -1104,10 +1125,10 @@
         <v>30</v>
       </c>
       <c r="C57" s="2">
-        <v>45580.48804522461</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>45580.488045224607</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -1115,10 +1136,10 @@
         <v>30</v>
       </c>
       <c r="C58" s="2">
-        <v>45580.48804522464</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>45580.488045224643</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -1126,10 +1147,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="2">
-        <v>45568.48804522467</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>45568.488045224673</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -1137,10 +1158,10 @@
         <v>12</v>
       </c>
       <c r="C60" s="2">
-        <v>45587.48804522472</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>45587.488045224723</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>45584.48804522476</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -1159,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="C62" s="2">
-        <v>45563.4880452248</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>45563.488045224803</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>45569.48804522484</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -1181,10 +1202,10 @@
         <v>41</v>
       </c>
       <c r="C64" s="2">
-        <v>45561.48804522488</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>45561.488045224884</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>32</v>
       </c>
@@ -1192,10 +1213,10 @@
         <v>29</v>
       </c>
       <c r="C65" s="2">
-        <v>45579.48804522491</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>45579.488045224913</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -1203,10 +1224,10 @@
         <v>20</v>
       </c>
       <c r="C66" s="2">
-        <v>45567.48804522496</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>45567.488045224964</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1238,7 @@
         <v>45582.488045225</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -1225,10 +1246,10 @@
         <v>23</v>
       </c>
       <c r="C68" s="2">
-        <v>45590.48804522504</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>45590.488045225044</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -1236,10 +1257,10 @@
         <v>24</v>
       </c>
       <c r="C69" s="2">
-        <v>45561.48804522507</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>45561.488045225073</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1247,10 +1268,10 @@
         <v>4</v>
       </c>
       <c r="C70" s="2">
-        <v>45573.48804522512</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>45573.488045225116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -1258,10 +1279,10 @@
         <v>24</v>
       </c>
       <c r="C71" s="2">
-        <v>45568.48804522515</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>45568.488045225153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -1269,10 +1290,10 @@
         <v>41</v>
       </c>
       <c r="C72" s="2">
-        <v>45585.4880452252</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>45585.488045225196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -1280,10 +1301,10 @@
         <v>28</v>
       </c>
       <c r="C73" s="2">
-        <v>45586.48804522523</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>45586.488045225233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -1291,10 +1312,10 @@
         <v>13</v>
       </c>
       <c r="C74" s="2">
-        <v>45568.48804522527</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>45568.488045225269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -1302,10 +1323,10 @@
         <v>8</v>
       </c>
       <c r="C75" s="2">
-        <v>45588.48804522531</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>45588.488045225313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -1313,10 +1334,10 @@
         <v>48</v>
       </c>
       <c r="C76" s="2">
-        <v>45562.48804522535</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>45562.488045225349</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -1324,10 +1345,10 @@
         <v>50</v>
       </c>
       <c r="C77" s="2">
-        <v>45567.48804522539</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>45567.488045225393</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -1335,10 +1356,10 @@
         <v>38</v>
       </c>
       <c r="C78" s="2">
-        <v>45579.48804522543</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>45579.488045225429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1346,10 +1367,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="2">
-        <v>45567.48804522547</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>45567.488045225473</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>27</v>
       </c>
@@ -1357,10 +1378,10 @@
         <v>25</v>
       </c>
       <c r="C80" s="2">
-        <v>45588.48804522551</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>45588.488045225509</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -1368,10 +1389,10 @@
         <v>35</v>
       </c>
       <c r="C81" s="2">
-        <v>45583.48804522555</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>45583.488045225553</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -1379,10 +1400,10 @@
         <v>48</v>
       </c>
       <c r="C82" s="2">
-        <v>45589.48804522559</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>45589.488045225589</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -1390,10 +1411,10 @@
         <v>25</v>
       </c>
       <c r="C83" s="2">
-        <v>45575.48804522563</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>45575.488045225633</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -1401,10 +1422,10 @@
         <v>46</v>
       </c>
       <c r="C84" s="2">
-        <v>45579.48804522567</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>45579.488045225669</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -1415,7 +1436,7 @@
         <v>45580.48804522572</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -1423,10 +1444,10 @@
         <v>32</v>
       </c>
       <c r="C86" s="2">
-        <v>45582.48804522575</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>45582.488045225749</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -1434,10 +1455,10 @@
         <v>9</v>
       </c>
       <c r="C87" s="2">
-        <v>45565.48804522579</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>45565.488045225793</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -1445,10 +1466,10 @@
         <v>22</v>
       </c>
       <c r="C88" s="2">
-        <v>45585.48804522584</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>45585.488045225837</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -1456,10 +1477,10 @@
         <v>16</v>
       </c>
       <c r="C89" s="2">
-        <v>45587.48804522587</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>45587.488045225873</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -1467,10 +1488,10 @@
         <v>26</v>
       </c>
       <c r="C90" s="2">
-        <v>45562.48804522592</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+        <v>45562.488045225917</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -1478,10 +1499,10 @@
         <v>18</v>
       </c>
       <c r="C91" s="2">
-        <v>45572.48804522595</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>45572.488045225953</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -1489,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="C92" s="2">
-        <v>45581.48804522598</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>45581.488045225982</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -1500,10 +1521,10 @@
         <v>48</v>
       </c>
       <c r="C93" s="2">
-        <v>45576.48804522603</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>45576.488045226033</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -1511,10 +1532,10 @@
         <v>32</v>
       </c>
       <c r="C94" s="2">
-        <v>45581.48804522606</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>45581.488045226062</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -1522,10 +1543,10 @@
         <v>8</v>
       </c>
       <c r="C95" s="2">
-        <v>45570.48804522611</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <v>45570.488045226113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -1533,10 +1554,10 @@
         <v>2</v>
       </c>
       <c r="C96" s="2">
-        <v>45571.48804522616</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <v>45571.488045226157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>28</v>
       </c>
@@ -1544,10 +1565,10 @@
         <v>26</v>
       </c>
       <c r="C97" s="2">
-        <v>45570.48804522619</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>45570.488045226193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1579,7 @@
         <v>45580.48804522623</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -1566,10 +1587,10 @@
         <v>6</v>
       </c>
       <c r="C99" s="2">
-        <v>45561.48804522626</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <v>45561.488045226259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1601,7 @@
         <v>45571.48804522631</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -1588,10 +1609,10 @@
         <v>10</v>
       </c>
       <c r="C101" s="2">
-        <v>45586.48804522635</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+        <v>45586.488045226353</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>28</v>
       </c>
@@ -1602,7 +1623,7 @@
         <v>45571.48804522639</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>32</v>
       </c>
@@ -1610,10 +1631,10 @@
         <v>7</v>
       </c>
       <c r="C103" s="2">
-        <v>45576.48804522643</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>45576.488045226433</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>28</v>
       </c>
@@ -1624,7 +1645,7 @@
         <v>45581.48804522647</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>27</v>
       </c>
@@ -1632,10 +1653,10 @@
         <v>15</v>
       </c>
       <c r="C105" s="2">
-        <v>45582.48804522651</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>45582.488045226513</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -1643,10 +1664,10 @@
         <v>12</v>
       </c>
       <c r="C106" s="2">
-        <v>45584.48804522654</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>45584.488045226542</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -1654,10 +1675,10 @@
         <v>2</v>
       </c>
       <c r="C107" s="2">
-        <v>45587.48804522659</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>45587.488045226593</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>21</v>
       </c>
@@ -1665,10 +1686,10 @@
         <v>8</v>
       </c>
       <c r="C108" s="2">
-        <v>45589.48804522662</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>45589.488045226622</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -1676,10 +1697,10 @@
         <v>25</v>
       </c>
       <c r="C109" s="2">
-        <v>45563.48804522667</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>45563.488045226673</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -1687,10 +1708,10 @@
         <v>18</v>
       </c>
       <c r="C110" s="2">
-        <v>45590.4880452267</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>45590.488045226703</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -1698,10 +1719,10 @@
         <v>24</v>
       </c>
       <c r="C111" s="2">
-        <v>45589.48804522675</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>45589.488045226753</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -1709,10 +1730,10 @@
         <v>15</v>
       </c>
       <c r="C112" s="2">
-        <v>45582.48804522678</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
+        <v>45582.488045226783</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -1720,10 +1741,10 @@
         <v>13</v>
       </c>
       <c r="C113" s="2">
-        <v>45585.48804522682</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+        <v>45585.488045226819</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -1731,10 +1752,10 @@
         <v>20</v>
       </c>
       <c r="C114" s="2">
-        <v>45573.48804522686</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <v>45573.488045226863</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -1742,10 +1763,10 @@
         <v>10</v>
       </c>
       <c r="C115" s="2">
-        <v>45576.4880452269</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <v>45576.488045226899</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>25</v>
       </c>
@@ -1753,10 +1774,10 @@
         <v>9</v>
       </c>
       <c r="C116" s="2">
-        <v>45568.48804522694</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>45568.488045226943</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -1764,10 +1785,10 @@
         <v>15</v>
       </c>
       <c r="C117" s="2">
-        <v>45563.48804522698</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+        <v>45563.488045226979</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>17</v>
       </c>
@@ -1775,10 +1796,10 @@
         <v>46</v>
       </c>
       <c r="C118" s="2">
-        <v>45579.48804522702</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
+        <v>45579.488045227023</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>21</v>
       </c>
@@ -1786,10 +1807,10 @@
         <v>43</v>
       </c>
       <c r="C119" s="2">
-        <v>45589.48804522706</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>45589.488045227059</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -1797,10 +1818,10 @@
         <v>29</v>
       </c>
       <c r="C120" s="2">
-        <v>45562.4880452271</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
+        <v>45562.488045227103</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -1808,10 +1829,10 @@
         <v>39</v>
       </c>
       <c r="C121" s="2">
-        <v>45586.48804522714</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
+        <v>45586.488045227139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -1819,10 +1840,10 @@
         <v>25</v>
       </c>
       <c r="C122" s="2">
-        <v>45580.48804522718</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
+        <v>45580.488045227183</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>14</v>
       </c>
@@ -1830,10 +1851,10 @@
         <v>34</v>
       </c>
       <c r="C123" s="2">
-        <v>45589.48804522721</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
+        <v>45589.488045227212</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -1841,10 +1862,10 @@
         <v>39</v>
       </c>
       <c r="C124" s="2">
-        <v>45577.48804522726</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
+        <v>45577.488045227263</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -1852,10 +1873,10 @@
         <v>38</v>
       </c>
       <c r="C125" s="2">
-        <v>45561.48804522731</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
+        <v>45561.488045227306</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -1866,7 +1887,7 @@
         <v>45567.48804522735</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -1874,10 +1895,10 @@
         <v>33</v>
       </c>
       <c r="C127" s="2">
-        <v>45566.48804522739</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>45566.488045227386</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>30</v>
       </c>
@@ -1888,7 +1909,7 @@
         <v>45582.48804522743</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -1896,10 +1917,10 @@
         <v>3</v>
       </c>
       <c r="C129" s="2">
-        <v>45586.48804522747</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+        <v>45586.488045227467</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1931,7 @@
         <v>45584.48804522751</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -1918,10 +1939,10 @@
         <v>50</v>
       </c>
       <c r="C131" s="2">
-        <v>45578.48804522756</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+        <v>45578.488045227561</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -1932,7 +1953,7 @@
         <v>45573.48804522759</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>21</v>
       </c>
@@ -1940,10 +1961,10 @@
         <v>4</v>
       </c>
       <c r="C133" s="2">
-        <v>45564.48804522763</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+        <v>45564.488045227627</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -1951,10 +1972,10 @@
         <v>18</v>
       </c>
       <c r="C134" s="2">
-        <v>45568.48804522766</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+        <v>45568.488045227663</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -1962,10 +1983,10 @@
         <v>6</v>
       </c>
       <c r="C135" s="2">
-        <v>45573.48804522771</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+        <v>45573.488045227707</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -1973,10 +1994,10 @@
         <v>41</v>
       </c>
       <c r="C136" s="2">
-        <v>45573.48804522774</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
+        <v>45573.488045227743</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>21</v>
       </c>
@@ -1984,10 +2005,10 @@
         <v>6</v>
       </c>
       <c r="C137" s="2">
-        <v>45589.48804522778</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+        <v>45589.488045227779</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>32</v>
       </c>
@@ -1995,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="2">
-        <v>45590.48804522782</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>45590.488045227823</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2027,10 @@
         <v>5</v>
       </c>
       <c r="C139" s="2">
-        <v>45568.48804522786</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+        <v>45568.488045227859</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>15</v>
       </c>
@@ -2017,10 +2038,10 @@
         <v>30</v>
       </c>
       <c r="C140" s="2">
-        <v>45576.4880452279</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+        <v>45576.488045227903</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>26</v>
       </c>
@@ -2028,10 +2049,10 @@
         <v>33</v>
       </c>
       <c r="C141" s="2">
-        <v>45583.48804522794</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>45583.488045227939</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>31</v>
       </c>
@@ -2039,10 +2060,10 @@
         <v>25</v>
       </c>
       <c r="C142" s="2">
-        <v>45563.48804522798</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
+        <v>45563.488045227983</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>26</v>
       </c>
@@ -2050,10 +2071,10 @@
         <v>13</v>
       </c>
       <c r="C143" s="2">
-        <v>45584.48804522802</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+        <v>45584.488045228019</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -2061,10 +2082,10 @@
         <v>22</v>
       </c>
       <c r="C144" s="2">
-        <v>45562.48804522806</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
+        <v>45562.488045228063</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>26</v>
       </c>
@@ -2075,7 +2096,7 @@
         <v>45572.4880452281</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -2083,10 +2104,10 @@
         <v>22</v>
       </c>
       <c r="C146" s="2">
-        <v>45568.48804522814</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
+        <v>45568.488045228143</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>13</v>
       </c>
@@ -2097,7 +2118,7 @@
         <v>45571.48804522818</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2129,7 @@
         <v>45590.48804522823</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -2116,10 +2137,10 @@
         <v>27</v>
       </c>
       <c r="C149" s="2">
-        <v>45587.48804522827</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
+        <v>45587.488045228267</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>15</v>
       </c>
@@ -2127,10 +2148,10 @@
         <v>34</v>
       </c>
       <c r="C150" s="2">
-        <v>45588.48804522833</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
+        <v>45588.488045228332</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -2138,10 +2159,10 @@
         <v>20</v>
       </c>
       <c r="C151" s="2">
-        <v>45564.48804522837</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
+        <v>45564.488045228369</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -2149,10 +2170,10 @@
         <v>43</v>
       </c>
       <c r="C152" s="2">
-        <v>45570.48804522841</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
+        <v>45570.488045228412</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -2160,10 +2181,10 @@
         <v>15</v>
       </c>
       <c r="C153" s="2">
-        <v>45573.48804522845</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
+        <v>45573.488045228449</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>29</v>
       </c>
@@ -2171,10 +2192,10 @@
         <v>41</v>
       </c>
       <c r="C154" s="2">
-        <v>45575.48804522849</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
+        <v>45575.488045228492</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>4</v>
       </c>
@@ -2182,10 +2203,10 @@
         <v>16</v>
       </c>
       <c r="C155" s="2">
-        <v>45586.48804522854</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
+        <v>45586.488045228543</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -2196,7 +2217,7 @@
         <v>45569.48804522858</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>29</v>
       </c>
@@ -2204,10 +2225,10 @@
         <v>43</v>
       </c>
       <c r="C157" s="2">
-        <v>45590.48804522861</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
+        <v>45590.488045228609</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -2215,10 +2236,10 @@
         <v>4</v>
       </c>
       <c r="C158" s="2">
-        <v>45561.48804522865</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
+        <v>45561.488045228652</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>25</v>
       </c>
@@ -2226,10 +2247,10 @@
         <v>20</v>
       </c>
       <c r="C159" s="2">
-        <v>45590.48804522869</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
+        <v>45590.488045228689</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>5</v>
       </c>
@@ -2237,10 +2258,10 @@
         <v>22</v>
       </c>
       <c r="C160" s="2">
-        <v>45586.48804522873</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+        <v>45586.488045228733</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>6</v>
       </c>
@@ -2248,10 +2269,10 @@
         <v>39</v>
       </c>
       <c r="C161" s="2">
-        <v>45584.48804522878</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
+        <v>45584.488045228783</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>29</v>
       </c>
@@ -2259,10 +2280,10 @@
         <v>8</v>
       </c>
       <c r="C162" s="2">
-        <v>45579.48804522881</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+        <v>45579.488045228813</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>5</v>
       </c>
@@ -2270,10 +2291,10 @@
         <v>48</v>
       </c>
       <c r="C163" s="2">
-        <v>45570.48804522884</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+        <v>45570.488045228842</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>16</v>
       </c>
@@ -2281,10 +2302,10 @@
         <v>20</v>
       </c>
       <c r="C164" s="2">
-        <v>45571.48804522889</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>45571.488045228893</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>21</v>
       </c>
@@ -2292,10 +2313,10 @@
         <v>39</v>
       </c>
       <c r="C165" s="2">
-        <v>45561.48804522892</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>45561.488045228922</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>20</v>
       </c>
@@ -2303,10 +2324,10 @@
         <v>34</v>
       </c>
       <c r="C166" s="2">
-        <v>45570.48804522897</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+        <v>45570.488045228973</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>27</v>
       </c>
@@ -2314,10 +2335,10 @@
         <v>27</v>
       </c>
       <c r="C167" s="2">
-        <v>45576.488045229</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+        <v>45576.488045229002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>31</v>
       </c>
@@ -2325,10 +2346,10 @@
         <v>47</v>
       </c>
       <c r="C168" s="2">
-        <v>45562.48804522904</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>45562.488045229038</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>20</v>
       </c>
@@ -2336,10 +2357,10 @@
         <v>19</v>
       </c>
       <c r="C169" s="2">
-        <v>45580.48804522907</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
+        <v>45580.488045229067</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -2347,10 +2368,10 @@
         <v>37</v>
       </c>
       <c r="C170" s="2">
-        <v>45561.48804522911</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
+        <v>45561.488045229111</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>19</v>
       </c>
@@ -2361,7 +2382,7 @@
         <v>45566.48804522914</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>20</v>
       </c>
@@ -2369,10 +2390,10 @@
         <v>35</v>
       </c>
       <c r="C172" s="2">
-        <v>45586.48804522918</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+        <v>45586.488045229184</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>5</v>
       </c>
@@ -2380,10 +2401,10 @@
         <v>13</v>
       </c>
       <c r="C173" s="2">
-        <v>45572.48804522923</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
+        <v>45572.488045229227</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>13</v>
       </c>
@@ -2391,10 +2412,10 @@
         <v>37</v>
       </c>
       <c r="C174" s="2">
-        <v>45583.48804522926</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>45583.488045229256</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>23</v>
       </c>
@@ -2402,10 +2423,10 @@
         <v>33</v>
       </c>
       <c r="C175" s="2">
-        <v>45589.48804522931</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>45589.488045229307</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>30</v>
       </c>
@@ -2413,10 +2434,10 @@
         <v>1</v>
       </c>
       <c r="C176" s="2">
-        <v>45581.48804522935</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
+        <v>45581.488045229351</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -2424,10 +2445,10 @@
         <v>9</v>
       </c>
       <c r="C177" s="2">
-        <v>45561.48804522939</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+        <v>45561.488045229387</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>30</v>
       </c>
@@ -2435,10 +2456,10 @@
         <v>38</v>
       </c>
       <c r="C178" s="2">
-        <v>45569.48804522943</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
+        <v>45569.488045229431</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>7</v>
       </c>
@@ -2446,10 +2467,10 @@
         <v>8</v>
       </c>
       <c r="C179" s="2">
-        <v>45586.48804522947</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
+        <v>45586.488045229467</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>31</v>
       </c>
@@ -2457,10 +2478,10 @@
         <v>8</v>
       </c>
       <c r="C180" s="2">
-        <v>45561.48804522951</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
+        <v>45561.488045229511</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>27</v>
       </c>
@@ -2468,10 +2489,10 @@
         <v>36</v>
       </c>
       <c r="C181" s="2">
-        <v>45585.48804522955</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+        <v>45585.488045229547</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>17</v>
       </c>
@@ -2479,10 +2500,10 @@
         <v>20</v>
       </c>
       <c r="C182" s="2">
-        <v>45569.4880452296</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+        <v>45569.488045229598</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>29</v>
       </c>
@@ -2490,10 +2511,10 @@
         <v>50</v>
       </c>
       <c r="C183" s="2">
-        <v>45574.48804522963</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
+        <v>45574.488045229627</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>19</v>
       </c>
@@ -2501,10 +2522,10 @@
         <v>10</v>
       </c>
       <c r="C184" s="2">
-        <v>45584.48804522966</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+        <v>45584.488045229657</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>20</v>
       </c>
@@ -2512,10 +2533,10 @@
         <v>39</v>
       </c>
       <c r="C185" s="2">
-        <v>45579.48804522971</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
+        <v>45579.488045229707</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>17</v>
       </c>
@@ -2523,10 +2544,10 @@
         <v>4</v>
       </c>
       <c r="C186" s="2">
-        <v>45576.48804522974</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
+        <v>45576.488045229737</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>13</v>
       </c>
@@ -2537,7 +2558,7 @@
         <v>45568.48804522978</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>32</v>
       </c>
@@ -2545,10 +2566,10 @@
         <v>24</v>
       </c>
       <c r="C188" s="2">
-        <v>45576.48804522982</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
+        <v>45576.488045229817</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>17</v>
       </c>
@@ -2559,7 +2580,7 @@
         <v>45589.48804522986</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>16</v>
       </c>
@@ -2567,10 +2588,10 @@
         <v>37</v>
       </c>
       <c r="C190" s="2">
-        <v>45579.4880452299</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
+        <v>45579.488045229897</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>27</v>
       </c>
@@ -2581,7 +2602,7 @@
         <v>45579.48804522994</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>13</v>
       </c>
@@ -2589,10 +2610,10 @@
         <v>11</v>
       </c>
       <c r="C192" s="2">
-        <v>45584.48804522999</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
+        <v>45584.488045229991</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>6</v>
       </c>
@@ -2603,7 +2624,7 @@
         <v>45562.48804523002</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>12</v>
       </c>
@@ -2611,10 +2632,10 @@
         <v>9</v>
       </c>
       <c r="C194" s="2">
-        <v>45586.48804523006</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
+        <v>45586.488045230057</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>14</v>
       </c>
@@ -2622,10 +2643,10 @@
         <v>20</v>
       </c>
       <c r="C195" s="2">
-        <v>45577.48804523009</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
+        <v>45577.488045230093</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -2633,10 +2654,10 @@
         <v>23</v>
       </c>
       <c r="C196" s="2">
-        <v>45575.48804523014</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
+        <v>45575.488045230137</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>28</v>
       </c>
@@ -2644,10 +2665,10 @@
         <v>43</v>
       </c>
       <c r="C197" s="2">
-        <v>45573.48804523017</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
+        <v>45573.488045230173</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>28</v>
       </c>
@@ -2655,10 +2676,10 @@
         <v>20</v>
       </c>
       <c r="C198" s="2">
-        <v>45585.48804523022</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
+        <v>45585.488045230217</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>23</v>
       </c>
@@ -2666,10 +2687,10 @@
         <v>26</v>
       </c>
       <c r="C199" s="2">
-        <v>45564.48804523025</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
+        <v>45564.488045230253</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -2677,10 +2698,10 @@
         <v>38</v>
       </c>
       <c r="C200" s="2">
-        <v>45561.4880452303</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
+        <v>45561.488045230297</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>13</v>
       </c>
@@ -2688,10 +2709,10 @@
         <v>34</v>
       </c>
       <c r="C201" s="2">
-        <v>45589.48804523033</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3">
+        <v>45589.488045230333</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>28</v>
       </c>
@@ -2702,7 +2723,7 @@
         <v>45582.48804523037</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>28</v>
       </c>
@@ -2710,10 +2731,10 @@
         <v>41</v>
       </c>
       <c r="C203" s="2">
-        <v>45577.48804523043</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
+        <v>45577.488045230428</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>19</v>
       </c>
@@ -2721,10 +2742,10 @@
         <v>43</v>
       </c>
       <c r="C204" s="2">
-        <v>45567.48804523046</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
+        <v>45567.488045230457</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>6</v>
       </c>
@@ -2732,10 +2753,10 @@
         <v>2</v>
       </c>
       <c r="C205" s="2">
-        <v>45568.48804523051</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
+        <v>45568.488045230508</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>26</v>
       </c>
@@ -2743,10 +2764,10 @@
         <v>16</v>
       </c>
       <c r="C206" s="2">
-        <v>45561.48804523054</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3">
+        <v>45561.488045230537</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -2754,10 +2775,10 @@
         <v>16</v>
       </c>
       <c r="C207" s="2">
-        <v>45578.48804523059</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
+        <v>45578.488045230588</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>18</v>
       </c>
@@ -2765,10 +2786,10 @@
         <v>18</v>
       </c>
       <c r="C208" s="2">
-        <v>45578.48804523062</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
+        <v>45578.488045230617</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>22</v>
       </c>
@@ -2776,10 +2797,10 @@
         <v>22</v>
       </c>
       <c r="C209" s="2">
-        <v>45567.48804523066</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
+        <v>45567.488045230661</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>26</v>
       </c>
@@ -2787,10 +2808,10 @@
         <v>16</v>
       </c>
       <c r="C210" s="2">
-        <v>45561.4880452307</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
+        <v>45561.488045230697</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>31</v>
       </c>
@@ -2798,10 +2819,10 @@
         <v>1</v>
       </c>
       <c r="C211" s="2">
-        <v>45573.48804523073</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
+        <v>45573.488045230733</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>29</v>
       </c>
@@ -2809,10 +2830,10 @@
         <v>22</v>
       </c>
       <c r="C212" s="2">
-        <v>45565.48804523076</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
+        <v>45565.488045230763</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>23</v>
       </c>
@@ -2820,10 +2841,10 @@
         <v>6</v>
       </c>
       <c r="C213" s="2">
-        <v>45569.48804523081</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
+        <v>45569.488045230813</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>18</v>
       </c>
@@ -2831,10 +2852,10 @@
         <v>50</v>
       </c>
       <c r="C214" s="2">
-        <v>45573.48804523084</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
+        <v>45573.488045230843</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>17</v>
       </c>
@@ -2842,10 +2863,10 @@
         <v>29</v>
       </c>
       <c r="C215" s="2">
-        <v>45582.48804523089</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
+        <v>45582.488045230893</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>8</v>
       </c>
@@ -2853,10 +2874,10 @@
         <v>44</v>
       </c>
       <c r="C216" s="2">
-        <v>45583.48804523092</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
+        <v>45583.488045230923</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>15</v>
       </c>
@@ -2864,10 +2885,10 @@
         <v>21</v>
       </c>
       <c r="C217" s="2">
-        <v>45564.48804523096</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
+        <v>45564.488045230959</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>4</v>
       </c>
@@ -2878,7 +2899,7 @@
         <v>45564.48804523101</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>10</v>
       </c>
@@ -2886,10 +2907,10 @@
         <v>23</v>
       </c>
       <c r="C219" s="2">
-        <v>45588.48804523104</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
+        <v>45588.488045231039</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>25</v>
       </c>
@@ -2897,10 +2918,10 @@
         <v>18</v>
       </c>
       <c r="C220" s="2">
-        <v>45577.48804523108</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
+        <v>45577.488045231083</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>9</v>
       </c>
@@ -2908,10 +2929,10 @@
         <v>16</v>
       </c>
       <c r="C221" s="2">
-        <v>45573.48804523113</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
+        <v>45573.488045231134</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>13</v>
       </c>
@@ -2919,10 +2940,10 @@
         <v>32</v>
       </c>
       <c r="C222" s="2">
-        <v>45573.48804523116</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
+        <v>45573.488045231163</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>21</v>
       </c>
@@ -2930,10 +2951,10 @@
         <v>27</v>
       </c>
       <c r="C223" s="2">
-        <v>45571.48804523119</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
+        <v>45571.488045231192</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>25</v>
       </c>
@@ -2941,10 +2962,10 @@
         <v>39</v>
       </c>
       <c r="C224" s="2">
-        <v>45589.48804523124</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
+        <v>45589.488045231243</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -2952,10 +2973,10 @@
         <v>14</v>
       </c>
       <c r="C225" s="2">
-        <v>45579.48804523127</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
+        <v>45579.488045231272</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>6</v>
       </c>
@@ -2963,10 +2984,10 @@
         <v>33</v>
       </c>
       <c r="C226" s="2">
-        <v>45577.48804523132</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
+        <v>45577.488045231323</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>7</v>
       </c>
@@ -2974,10 +2995,10 @@
         <v>9</v>
       </c>
       <c r="C227" s="2">
-        <v>45573.48804523135</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
+        <v>45573.488045231352</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>31</v>
       </c>
@@ -2985,10 +3006,10 @@
         <v>30</v>
       </c>
       <c r="C228" s="2">
-        <v>45568.4880452314</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
+        <v>45568.488045231403</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>19</v>
       </c>
@@ -2996,10 +3017,10 @@
         <v>38</v>
       </c>
       <c r="C229" s="2">
-        <v>45582.48804523143</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
+        <v>45582.488045231432</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>23</v>
       </c>
@@ -3007,10 +3028,10 @@
         <v>22</v>
       </c>
       <c r="C230" s="2">
-        <v>45587.48804523148</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
+        <v>45587.488045231483</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>18</v>
       </c>
@@ -3018,10 +3039,10 @@
         <v>44</v>
       </c>
       <c r="C231" s="2">
-        <v>45589.48804523152</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
+        <v>45589.488045231519</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>28</v>
       </c>
@@ -3029,10 +3050,10 @@
         <v>45</v>
       </c>
       <c r="C232" s="2">
-        <v>45573.48804523156</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
+        <v>45573.488045231563</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>27</v>
       </c>
@@ -3040,10 +3061,10 @@
         <v>4</v>
       </c>
       <c r="C233" s="2">
-        <v>45586.4880452316</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
+        <v>45586.488045231599</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>18</v>
       </c>
@@ -3051,10 +3072,10 @@
         <v>13</v>
       </c>
       <c r="C234" s="2">
-        <v>45566.48804523163</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
+        <v>45566.488045231628</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>15</v>
       </c>
@@ -3062,10 +3083,10 @@
         <v>27</v>
       </c>
       <c r="C235" s="2">
-        <v>45563.48804523169</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
+        <v>45563.488045231687</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>13</v>
       </c>
@@ -3073,10 +3094,10 @@
         <v>36</v>
       </c>
       <c r="C236" s="2">
-        <v>45576.48804523172</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
+        <v>45576.488045231723</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -3084,10 +3105,10 @@
         <v>49</v>
       </c>
       <c r="C237" s="2">
-        <v>45579.48804523177</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
+        <v>45579.488045231767</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>19</v>
       </c>
@@ -3095,10 +3116,10 @@
         <v>18</v>
       </c>
       <c r="C238" s="2">
-        <v>45581.4880452318</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
+        <v>45581.488045231803</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>31</v>
       </c>
@@ -3106,10 +3127,10 @@
         <v>14</v>
       </c>
       <c r="C239" s="2">
-        <v>45565.48804523185</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
+        <v>45565.488045231847</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>22</v>
       </c>
@@ -3117,10 +3138,10 @@
         <v>17</v>
       </c>
       <c r="C240" s="2">
-        <v>45581.48804523204</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
+        <v>45581.488045232043</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>13</v>
       </c>
@@ -3128,10 +3149,10 @@
         <v>10</v>
       </c>
       <c r="C241" s="2">
-        <v>45563.48804523207</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
+        <v>45563.488045232072</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>24</v>
       </c>
@@ -3139,10 +3160,10 @@
         <v>31</v>
       </c>
       <c r="C242" s="2">
-        <v>45567.48804523211</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
+        <v>45567.488045232109</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>14</v>
       </c>
@@ -3150,10 +3171,10 @@
         <v>49</v>
       </c>
       <c r="C243" s="2">
-        <v>45587.48804523215</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
+        <v>45587.488045232152</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>19</v>
       </c>
@@ -3161,10 +3182,10 @@
         <v>47</v>
       </c>
       <c r="C244" s="2">
-        <v>45568.48804523219</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
+        <v>45568.488045232189</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>12</v>
       </c>
@@ -3172,10 +3193,10 @@
         <v>33</v>
       </c>
       <c r="C245" s="2">
-        <v>45587.48804523222</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
+        <v>45587.488045232218</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>23</v>
       </c>
@@ -3183,10 +3204,10 @@
         <v>7</v>
       </c>
       <c r="C246" s="2">
-        <v>45580.48804523225</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
+        <v>45580.488045232247</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>4</v>
       </c>
@@ -3197,7 +3218,7 @@
         <v>45586.48804523229</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>25</v>
       </c>
@@ -3205,10 +3226,10 @@
         <v>20</v>
       </c>
       <c r="C248" s="2">
-        <v>45585.48804523233</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
+        <v>45585.488045232327</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>31</v>
       </c>
@@ -3219,7 +3240,7 @@
         <v>45590.48804523237</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>17</v>
       </c>
@@ -3227,10 +3248,10 @@
         <v>14</v>
       </c>
       <c r="C250" s="2">
-        <v>45563.48804523241</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
+        <v>45563.488045232407</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>9</v>
       </c>
@@ -3238,10 +3259,10 @@
         <v>46</v>
       </c>
       <c r="C251" s="2">
-        <v>45577.48804523245</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
+        <v>45577.488045232451</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>5</v>
       </c>
@@ -3249,10 +3270,10 @@
         <v>35</v>
       </c>
       <c r="C252" s="2">
-        <v>45574.48804523249</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
+        <v>45574.488045232487</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>20</v>
       </c>
@@ -3260,10 +3281,10 @@
         <v>25</v>
       </c>
       <c r="C253" s="2">
-        <v>45582.48804523254</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
+        <v>45582.488045232538</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>7</v>
       </c>
@@ -3271,10 +3292,10 @@
         <v>28</v>
       </c>
       <c r="C254" s="2">
-        <v>45567.48804523257</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
+        <v>45567.488045232567</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>17</v>
       </c>
@@ -3282,10 +3303,10 @@
         <v>35</v>
       </c>
       <c r="C255" s="2">
-        <v>45585.48804523262</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
+        <v>45585.488045232618</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>23</v>
       </c>
@@ -3293,10 +3314,10 @@
         <v>17</v>
       </c>
       <c r="C256" s="2">
-        <v>45577.48804523265</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
+        <v>45577.488045232647</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>16</v>
       </c>
@@ -3304,10 +3325,10 @@
         <v>7</v>
       </c>
       <c r="C257" s="2">
-        <v>45580.4880452327</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
+        <v>45580.488045232698</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>7</v>
       </c>
@@ -3315,10 +3336,10 @@
         <v>23</v>
       </c>
       <c r="C258" s="2">
-        <v>45569.48804523273</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
+        <v>45569.488045232727</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>11</v>
       </c>
@@ -3326,10 +3347,10 @@
         <v>16</v>
       </c>
       <c r="C259" s="2">
-        <v>45562.48804523276</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
+        <v>45562.488045232763</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>3</v>
       </c>
@@ -3337,10 +3358,10 @@
         <v>46</v>
       </c>
       <c r="C260" s="2">
-        <v>45581.48804523281</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
+        <v>45581.488045232807</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>6</v>
       </c>
@@ -3348,10 +3369,10 @@
         <v>45</v>
       </c>
       <c r="C261" s="2">
-        <v>45568.48804523285</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
+        <v>45568.488045232851</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>19</v>
       </c>
@@ -3359,10 +3380,10 @@
         <v>36</v>
       </c>
       <c r="C262" s="2">
-        <v>45563.48804523289</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
+        <v>45563.488045232887</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>3</v>
       </c>
@@ -3370,10 +3391,10 @@
         <v>34</v>
       </c>
       <c r="C263" s="2">
-        <v>45563.48804523294</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
+        <v>45563.488045232938</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>8</v>
       </c>
@@ -3381,10 +3402,10 @@
         <v>32</v>
       </c>
       <c r="C264" s="2">
-        <v>45580.48804523297</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
+        <v>45580.488045232967</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>21</v>
       </c>
@@ -3392,10 +3413,10 @@
         <v>16</v>
       </c>
       <c r="C265" s="2">
-        <v>45569.48804523302</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
+        <v>45569.488045233018</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>6</v>
       </c>
@@ -3403,10 +3424,10 @@
         <v>20</v>
       </c>
       <c r="C266" s="2">
-        <v>45567.48804523305</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
+        <v>45567.488045233047</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>5</v>
       </c>
@@ -3414,10 +3435,10 @@
         <v>25</v>
       </c>
       <c r="C267" s="2">
-        <v>45577.48804523309</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
+        <v>45577.488045233091</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>28</v>
       </c>
@@ -3425,10 +3446,10 @@
         <v>4</v>
       </c>
       <c r="C268" s="2">
-        <v>45563.48804523313</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
+        <v>45563.488045233127</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>21</v>
       </c>
@@ -3436,10 +3457,10 @@
         <v>30</v>
       </c>
       <c r="C269" s="2">
-        <v>45577.48804523317</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
+        <v>45577.488045233171</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>19</v>
       </c>
@@ -3447,10 +3468,10 @@
         <v>19</v>
       </c>
       <c r="C270" s="2">
-        <v>45562.48804523321</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
+        <v>45562.488045233207</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>16</v>
       </c>
@@ -3458,10 +3479,10 @@
         <v>23</v>
       </c>
       <c r="C271" s="2">
-        <v>45572.48804523325</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3">
+        <v>45572.488045233251</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>18</v>
       </c>
@@ -3469,10 +3490,10 @@
         <v>7</v>
       </c>
       <c r="C272" s="2">
-        <v>45581.4880452333</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3">
+        <v>45581.488045233302</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>28</v>
       </c>
@@ -3480,10 +3501,10 @@
         <v>47</v>
       </c>
       <c r="C273" s="2">
-        <v>45579.48804523333</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
+        <v>45579.488045233331</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>25</v>
       </c>
@@ -3491,10 +3512,10 @@
         <v>33</v>
       </c>
       <c r="C274" s="2">
-        <v>45565.48804523338</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
+        <v>45565.488045233382</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>30</v>
       </c>
@@ -3502,10 +3523,10 @@
         <v>11</v>
       </c>
       <c r="C275" s="2">
-        <v>45578.48804523343</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3">
+        <v>45578.488045233433</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>29</v>
       </c>
@@ -3513,10 +3534,10 @@
         <v>27</v>
       </c>
       <c r="C276" s="2">
-        <v>45576.48804523346</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3">
+        <v>45576.488045233462</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>24</v>
       </c>
@@ -3524,10 +3545,10 @@
         <v>11</v>
       </c>
       <c r="C277" s="2">
-        <v>45586.4880452335</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3">
+        <v>45586.488045233498</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>5</v>
       </c>
@@ -3535,10 +3556,10 @@
         <v>30</v>
       </c>
       <c r="C278" s="2">
-        <v>45566.48804523354</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
+        <v>45566.488045233542</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>31</v>
       </c>
@@ -3546,10 +3567,10 @@
         <v>49</v>
       </c>
       <c r="C279" s="2">
-        <v>45563.48804523358</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
+        <v>45563.488045233578</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>12</v>
       </c>
@@ -3557,10 +3578,10 @@
         <v>48</v>
       </c>
       <c r="C280" s="2">
-        <v>45578.48804523362</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3">
+        <v>45578.488045233622</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>30</v>
       </c>
@@ -3568,10 +3589,10 @@
         <v>4</v>
       </c>
       <c r="C281" s="2">
-        <v>45567.48804523367</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3">
+        <v>45567.488045233673</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>3</v>
       </c>
@@ -3579,10 +3600,10 @@
         <v>19</v>
       </c>
       <c r="C282" s="2">
-        <v>45584.4880452337</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3">
+        <v>45584.488045233702</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>21</v>
       </c>
@@ -3590,10 +3611,10 @@
         <v>25</v>
       </c>
       <c r="C283" s="2">
-        <v>45562.48804523374</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3">
+        <v>45562.488045233738</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>5</v>
       </c>
@@ -3601,10 +3622,10 @@
         <v>46</v>
       </c>
       <c r="C284" s="2">
-        <v>45588.48804523377</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3">
+        <v>45588.488045233767</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>18</v>
       </c>
@@ -3612,10 +3633,10 @@
         <v>32</v>
       </c>
       <c r="C285" s="2">
-        <v>45587.48804523382</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3">
+        <v>45587.488045233818</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>21</v>
       </c>
@@ -3623,10 +3644,10 @@
         <v>38</v>
       </c>
       <c r="C286" s="2">
-        <v>45567.48804523385</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3">
+        <v>45567.488045233848</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>32</v>
       </c>
@@ -3634,10 +3655,10 @@
         <v>39</v>
       </c>
       <c r="C287" s="2">
-        <v>45576.4880452339</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3">
+        <v>45576.488045233898</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>29</v>
       </c>
@@ -3645,10 +3666,10 @@
         <v>17</v>
       </c>
       <c r="C288" s="2">
-        <v>45583.48804523393</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3">
+        <v>45583.488045233928</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>19</v>
       </c>
@@ -3656,10 +3677,10 @@
         <v>42</v>
       </c>
       <c r="C289" s="2">
-        <v>45577.48804523397</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3">
+        <v>45577.488045233971</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>25</v>
       </c>
@@ -3667,10 +3688,10 @@
         <v>1</v>
       </c>
       <c r="C290" s="2">
-        <v>45562.48804523401</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3">
+        <v>45562.488045234008</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>31</v>
       </c>
@@ -3678,10 +3699,10 @@
         <v>27</v>
       </c>
       <c r="C291" s="2">
-        <v>45578.48804523405</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3">
+        <v>45578.488045234051</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>11</v>
       </c>
@@ -3689,10 +3710,10 @@
         <v>21</v>
       </c>
       <c r="C292" s="2">
-        <v>45571.48804523409</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3">
+        <v>45571.488045234088</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>31</v>
       </c>
@@ -3700,10 +3721,10 @@
         <v>48</v>
       </c>
       <c r="C293" s="2">
-        <v>45580.48804523413</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3">
+        <v>45580.488045234131</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>4</v>
       </c>
@@ -3711,10 +3732,10 @@
         <v>13</v>
       </c>
       <c r="C294" s="2">
-        <v>45585.48804523417</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3">
+        <v>45585.488045234168</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>22</v>
       </c>
@@ -3722,10 +3743,10 @@
         <v>24</v>
       </c>
       <c r="C295" s="2">
-        <v>45589.48804523421</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3">
+        <v>45589.488045234211</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>19</v>
       </c>
@@ -3733,10 +3754,10 @@
         <v>1</v>
       </c>
       <c r="C296" s="2">
-        <v>45565.48804523425</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3">
+        <v>45565.488045234248</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>29</v>
       </c>
@@ -3744,10 +3765,10 @@
         <v>1</v>
       </c>
       <c r="C297" s="2">
-        <v>45577.48804523428</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3">
+        <v>45577.488045234277</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>21</v>
       </c>
@@ -3755,10 +3776,10 @@
         <v>7</v>
       </c>
       <c r="C298" s="2">
-        <v>45588.48804523433</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3">
+        <v>45588.488045234328</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>5</v>
       </c>
@@ -3766,10 +3787,10 @@
         <v>1</v>
       </c>
       <c r="C299" s="2">
-        <v>45570.48804523436</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3">
+        <v>45570.488045234357</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>3</v>
       </c>
@@ -3777,10 +3798,10 @@
         <v>47</v>
       </c>
       <c r="C300" s="2">
-        <v>45583.48804523441</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3">
+        <v>45583.488045234408</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>32</v>
       </c>
@@ -3788,7 +3809,7 @@
         <v>28</v>
       </c>
       <c r="C301" s="2">
-        <v>45583.48804523444</v>
+        <v>45583.488045234437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>